<commit_message>
Added table and code to report
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gcn_sampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A07507-235F-40BA-B841-CC76A3BAEF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548F023F-5B79-48BE-A056-84AD42DFBA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D4CE9A1-03AD-4904-84AE-862576010658}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7D4CE9A1-03AD-4904-84AE-862576010658}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,15 +127,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE769AF-F18B-41C8-9864-36CCB4C1493D}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -483,18 +482,18 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.82799999999999996</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.69199999999999995</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>0.77</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -503,18 +502,18 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.77</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.624</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>0.70899999999999996</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
@@ -523,18 +522,18 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.80100000000000005</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>0.69</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>0.76200000000000001</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
@@ -543,18 +542,18 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.62</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>0.7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>0.76400000000000001</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
@@ -563,18 +562,18 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.58299999999999996</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.29699999999999999</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>0.18</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -583,18 +582,18 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.76900000000000002</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.42699999999999999</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>0.59199999999999997</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
@@ -603,18 +602,18 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>0.78700000000000003</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>0.68400000000000005</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>0.76700000000000002</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
@@ -623,18 +622,18 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.81499999999999995</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>0.69599999999999995</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>0.78</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
@@ -643,18 +642,18 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.77300000000000002</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>0.66300000000000003</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>0.73199999999999998</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
@@ -663,18 +662,18 @@
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0.81</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>0.70899999999999996</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>0.77600000000000002</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
@@ -683,18 +682,18 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>0.55100000000000005</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>0.71699999999999997</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>0.75800000000000001</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
@@ -703,18 +702,18 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.434</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>0.50600000000000001</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>0.18</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
@@ -723,18 +722,18 @@
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>0.70099999999999996</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>0.51700000000000002</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>0.52600000000000002</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
@@ -743,18 +742,18 @@
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.81499999999999995</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>0.68100000000000005</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>0.73199999999999998</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
@@ -763,13 +762,13 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>0.82499999999999996</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>0.71</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>0.77900000000000003</v>
       </c>
     </row>
@@ -780,16 +779,16 @@
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>0.78800000000000003</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>0.68300000000000005</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>0.76400000000000001</v>
       </c>
-      <c r="G17" s="6"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
@@ -798,13 +797,13 @@
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>0.79300000000000004</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>0.72</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>0.78600000000000003</v>
       </c>
     </row>
@@ -815,13 +814,13 @@
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>0.625</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>0.71499999999999997</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>0.76300000000000001</v>
       </c>
     </row>
@@ -832,13 +831,13 @@
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>0.69399999999999995</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>0.193</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>0.51700000000000002</v>
       </c>
     </row>
@@ -849,13 +848,13 @@
       <c r="B21">
         <v>3</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>0.67</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>0.53</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>0.56100000000000005</v>
       </c>
     </row>
@@ -866,13 +865,13 @@
       <c r="B22">
         <v>3</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>0.81</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>0.68899999999999995</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>0.75</v>
       </c>
     </row>
@@ -883,16 +882,16 @@
       <c r="B23">
         <v>4</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>0.81299999999999994</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>0.69599999999999995</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>0.752</v>
       </c>
-      <c r="H23" s="3"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
@@ -901,16 +900,16 @@
       <c r="B24">
         <v>4</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>0.77300000000000002</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>0.63700000000000001</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>0.72899999999999998</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
@@ -919,16 +918,16 @@
       <c r="B25">
         <v>4</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>0.82599999999999996</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>0.71</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>0.76100000000000001</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
@@ -937,16 +936,16 @@
       <c r="B26">
         <v>4</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>0.57699999999999996</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>0.70499999999999996</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>0.76600000000000001</v>
       </c>
-      <c r="H26" s="3"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
@@ -955,16 +954,16 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>0.72299999999999998</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>0.371</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>0.18</v>
       </c>
-      <c r="H27" s="3"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
@@ -973,16 +972,16 @@
       <c r="B28">
         <v>4</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>0.68700000000000006</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>0.54500000000000004</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>0.54800000000000004</v>
       </c>
-      <c r="H28" s="3"/>
+      <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
@@ -991,21 +990,24 @@
       <c r="B29">
         <v>4</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>0.78300000000000003</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>0.69</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>0.76400000000000001</v>
       </c>
-      <c r="H29" s="4"/>
+      <c r="H29" s="3"/>
+      <c r="I29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
@@ -1020,29 +1022,29 @@
       <c r="D31" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <f>AVERAGEIF($A$2:$A$29, "=Baseline",C$2:C$29)</f>
         <v>0.82024999999999992</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <f>AVERAGEIF($A$2:$A$29, "=Baseline",D$2:D$29)</f>
         <v>0.6984999999999999</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <f>AVERAGEIF($A$2:$A$29, "=Baseline",E$2:E$29)</f>
         <v>0.7702500000000001</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
@@ -1060,29 +1062,29 @@
         <f t="shared" si="0"/>
         <v>0.73350000000000004</v>
       </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="6">
         <f>AVERAGEIF($A$2:$A$29, "=ClusterGCN",C$2:C$29)</f>
         <v>0.80750000000000011</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="6">
         <f t="shared" ref="C34:D34" si="1">AVERAGEIF($A$2:$A$29, "=ClusterGCN",D$2:D$29)</f>
         <v>0.70724999999999993</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <f t="shared" si="1"/>
         <v>0.77124999999999999</v>
       </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
@@ -1092,17 +1094,17 @@
         <f>AVERAGEIF($A$2:$A$29, "=GraphSAGE",C$2:C$29)</f>
         <v>0.59325000000000006</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="6">
         <f t="shared" ref="C35:D35" si="2">AVERAGEIF($A$2:$A$29, "=GraphSAGE",D$2:D$29)</f>
         <v>0.70924999999999994</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="6">
         <f t="shared" si="2"/>
         <v>0.76275000000000004</v>
       </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
@@ -1120,9 +1122,9 @@
         <f t="shared" si="3"/>
         <v>0.26424999999999998</v>
       </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
@@ -1145,7 +1147,7 @@
       <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="6">
         <f>AVERAGEIF($A$2:$A$29, "=GraphSAINT Random Walk Sampler",C$2:C$29)</f>
         <v>0.79874999999999996</v>
       </c>

</xml_diff>